<commit_message>
ok arreglados tabla de valores y matriz normales
</commit_message>
<xml_diff>
--- a/src/tp_aproximacion/tp aproximacion v2.xlsx
+++ b/src/tp_aproximacion/tp aproximacion v2.xlsx
@@ -407,11 +407,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52852992"/>
-        <c:axId val="52872320"/>
+        <c:axId val="111000192"/>
+        <c:axId val="111010560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52852992"/>
+        <c:axId val="111000192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -443,12 +443,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52872320"/>
+        <c:crossAx val="111010560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52872320"/>
+        <c:axId val="111010560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52852992"/>
+        <c:crossAx val="111000192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2622,14 +2622,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
   </cols>
@@ -2934,7 +2935,7 @@
         <v>42.875</v>
       </c>
       <c r="H7" s="16">
-        <f t="shared" ref="H3:H13" si="9">B7^4</f>
+        <f t="shared" ref="H7:H13" si="9">B7^4</f>
         <v>150.0625</v>
       </c>
       <c r="I7" s="16">
@@ -3245,7 +3246,7 @@
         <v>42.7</v>
       </c>
       <c r="C14" s="16">
-        <f t="shared" ref="C14:H14" si="10">SUM(C2:C13)</f>
+        <f t="shared" ref="C14" si="10">SUM(C2:C13)</f>
         <v>78.822000000000003</v>
       </c>
       <c r="D14" s="16">

</xml_diff>